<commit_message>
update data lab 3
</commit_message>
<xml_diff>
--- a/Session3/ExampleLab3.xlsx
+++ b/Session3/ExampleLab3.xlsx
@@ -179,7 +179,7 @@
     <t>HouseholdSize</t>
   </si>
   <si>
-    <t xml:space="preserve">3 </t>
+    <t>l</t>
   </si>
 </sst>
 </file>
@@ -518,7 +518,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -600,9 +600,6 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>22</v>
-      </c>
       <c r="C5" t="s">
         <v>34</v>
       </c>
@@ -847,8 +844,8 @@
       <c r="D19" t="s">
         <v>46</v>
       </c>
-      <c r="E19">
-        <v>1</v>
+      <c r="E19" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1017,9 +1014,7 @@
       <c r="D29" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">

</xml_diff>